<commit_message>
Add: name field. Add: logging in starrynift, minor fixes
</commit_message>
<xml_diff>
--- a/wallet_data.xlsx
+++ b/wallet_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rgalyeon/soft_rgalyeon/starrynift/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA6FC6F-771B-2647-80B8-BD2C1DF40FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0923E85-E40A-E84E-9B61-C774302EBEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>address</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>api_key;secret;api_password</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name1</t>
   </si>
 </sst>
 </file>
@@ -110,11 +116,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,69 +429,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="36.83203125" customWidth="1"/>
+    <col min="6" max="6" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>